<commit_message>
added new row to university_police_actions sheets
</commit_message>
<xml_diff>
--- a/docs/data-cleaning-requests/university-police-actions/university_police_actions_all.xlsx
+++ b/docs/data-cleaning-requests/university-police-actions/university_police_actions_all.xlsx
@@ -352,7 +352,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -483,20 +483,30 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Number of events with neither university response nor police coding</t>
+          <t>Number of events with both any university response coding and any police coding</t>
         </is>
       </c>
       <c r="B13">
-        <v>3299</v>
+        <v>360</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>Number of events with neither university response nor police coding</t>
+        </is>
+      </c>
+      <c r="B14">
+        <v>3299</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
           <t>Total number of protests</t>
         </is>
       </c>
-      <c r="B14">
+      <c r="B15">
         <v>5560</v>
       </c>
     </row>

</xml_diff>